<commit_message>
feat: add preco app
</commit_message>
<xml_diff>
--- a/static/models/modelo_tabloide.xlsx
+++ b/static/models/modelo_tabloide.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altaneiro.analista01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\web-comercial\static\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFCA889-881A-4668-A2EE-28A4D2668032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F560D5D-E82B-458F-92DA-9E0608C8A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="2880" windowWidth="24015" windowHeight="11295" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelas" sheetId="2" state="hidden" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Excluídos!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Todos!$A$1:$H$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Todos!$A$1:$I$124</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Excluídos!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Todos!$1:$1</definedName>
   </definedNames>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>GTIN</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>PREÇO DESCONTO CLIENTE+</t>
+  </si>
+  <si>
+    <t>PREÇO APP</t>
   </si>
 </sst>
 </file>
@@ -317,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -335,6 +338,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1103,13 +1109,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:K124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="A2:H2"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1120,13 +1126,14 @@
     <col min="4" max="4" width="17.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27" style="5" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="6" customWidth="1"/>
-    <col min="9" max="10" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" hidden="1"/>
+    <col min="7" max="7" width="26.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="22" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="6" customWidth="1"/>
+    <col min="10" max="11" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1148,25 +1155,28 @@
       <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1276,8 +1286,8 @@
     <row r="123" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="124" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:H124" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <conditionalFormatting sqref="A2:H1048576">
+  <autoFilter ref="A1:I124" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <conditionalFormatting sqref="A2:I1048576">
     <cfRule type="expression" dxfId="5" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -1290,7 +1300,7 @@
       <formula>COLUMN()=6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H1048576">
+  <conditionalFormatting sqref="G2:I1048576">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>COLUMN()&gt;6</formula>
     </cfRule>

</xml_diff>

<commit_message>
correcao gtins e modelos
</commit_message>
<xml_diff>
--- a/static/models/modelo_tabloide.xlsx
+++ b/static/models/modelo_tabloide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\web-comercial\static\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F560D5D-E82B-458F-92DA-9E0608C8A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6F2E40-B210-462F-A7B5-3C7A7E250879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="2880" windowWidth="24015" windowHeight="11295" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelas" sheetId="2" state="hidden" r:id="rId1"/>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{BA328680-A01B-4707-980E-3819F7F905AD}">
       <text>
         <r>
           <rPr>
@@ -1109,13 +1109,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K124"/>
+  <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1127,10 +1127,11 @@
     <col min="5" max="5" width="19.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" style="5" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="22" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="22" style="5" customWidth="1"/>
     <col min="10" max="11" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" hidden="1"/>
+    <col min="12" max="12" width="0" style="1" hidden="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1155,11 +1156,11 @@
       <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>